<commit_message>
corrected values in ion database
</commit_message>
<xml_diff>
--- a/aqpolypy/salt/paramsPM.xlsx
+++ b/aqpolypy/salt/paramsPM.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trvsst\Research\aqpolypy\aqpolypy\salt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56E57F4-F601-4912-B8FB-5EADB1B9A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13372E3C-1097-4905-A855-2C42049CB257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>HCl</t>
   </si>
@@ -379,6 +388,15 @@
   </si>
   <si>
     <t>nm</t>
+  </si>
+  <si>
+    <t>NaH2PO4</t>
+  </si>
+  <si>
+    <t>KI</t>
+  </si>
+  <si>
+    <t>RbNO2</t>
   </si>
 </sst>
 </file>
@@ -696,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -834,7 +852,7 @@
         <v>0.29310000000000003</v>
       </c>
       <c r="D5">
-        <v>8.1900000000000001E-2</v>
+        <v>8.1899999999999994E-3</v>
       </c>
       <c r="E5">
         <v>5.5</v>
@@ -1060,7 +1078,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.97299999999999998</v>
+        <v>9.7299999999999998E-2</v>
       </c>
       <c r="C13">
         <v>0.27910000000000001</v>
@@ -1153,7 +1171,7 @@
         <v>0.2455</v>
       </c>
       <c r="D16">
-        <v>4.0000000000000001E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="E16">
         <v>3.5</v>
@@ -1292,13 +1310,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-5.33E-2</v>
+        <v>6.7999999999999996E-3</v>
       </c>
       <c r="C21">
-        <v>3.9600000000000003E-2</v>
+        <v>0.17829999999999999</v>
       </c>
       <c r="D21">
-        <v>7.9500000000000005E-3</v>
+        <v>-7.2000000000000005E-4</v>
       </c>
       <c r="E21">
         <v>6</v>
@@ -1318,16 +1336,16 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="B22">
-        <v>-5.2600000000000001E-2</v>
+        <v>-5.33E-2</v>
       </c>
       <c r="C22">
-        <v>0.1104</v>
+        <v>3.9600000000000003E-2</v>
       </c>
       <c r="D22">
-        <v>1.54E-2</v>
+        <v>7.9500000000000005E-3</v>
       </c>
       <c r="E22">
         <v>6</v>
@@ -1347,16 +1365,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
-        <v>-2.52E-2</v>
+        <v>-5.2600000000000001E-2</v>
       </c>
       <c r="C23">
-        <v>0.18240000000000001</v>
+        <v>0.1104</v>
       </c>
       <c r="D23">
-        <v>2.0999999999999999E-3</v>
+        <v>1.54E-2</v>
       </c>
       <c r="E23">
         <v>6</v>
@@ -1376,19 +1394,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
-        <v>8.0890000000000004E-2</v>
+        <v>-2.52E-2</v>
       </c>
       <c r="C24">
-        <v>0.2021</v>
+        <v>0.18240000000000001</v>
       </c>
       <c r="D24">
-        <v>9.3000000000000005E-4</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1405,19 +1423,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
-        <v>4.8349999999999997E-2</v>
+        <v>8.0890000000000004E-2</v>
       </c>
       <c r="C25">
-        <v>0.2122</v>
+        <v>0.2021</v>
       </c>
       <c r="D25">
-        <v>-8.4000000000000003E-4</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="E25">
-        <v>4.8</v>
+        <v>2</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1434,19 +1452,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>5.6899999999999999E-2</v>
+        <v>4.8349999999999997E-2</v>
       </c>
       <c r="C26">
-        <v>0.22120000000000001</v>
+        <v>0.2122</v>
       </c>
       <c r="D26">
-        <v>-1.8E-3</v>
+        <v>-8.4000000000000003E-4</v>
       </c>
       <c r="E26">
-        <v>5.5</v>
+        <v>4.8</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1463,16 +1481,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
-        <v>0.1298</v>
+        <v>5.6899999999999999E-2</v>
       </c>
       <c r="C27">
-        <v>0.32</v>
+        <v>0.22120000000000001</v>
       </c>
       <c r="D27">
-        <v>4.1000000000000003E-3</v>
+        <v>-1.8E-3</v>
       </c>
       <c r="E27">
         <v>5.5</v>
@@ -1492,19 +1510,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="B28">
-        <v>4.1599999999999998E-2</v>
+        <v>7.46E-2</v>
       </c>
       <c r="C28">
-        <v>0.23019999999999999</v>
+        <v>0.25169999999999998</v>
       </c>
       <c r="D28">
-        <v>-2.5200000000000001E-3</v>
+        <v>-4.1399999999999996E-3</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1521,19 +1539,19 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29">
-        <v>0.151</v>
+        <v>0.1298</v>
       </c>
       <c r="C29">
-        <v>1.4999999999999999E-2</v>
+        <v>0.32</v>
       </c>
       <c r="D29">
-        <v>6.9999999999999999E-4</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1550,19 +1568,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30">
-        <v>-8.1600000000000006E-2</v>
+        <v>4.1599999999999998E-2</v>
       </c>
       <c r="C30">
-        <v>4.9399999999999999E-2</v>
+        <v>0.23019999999999999</v>
       </c>
       <c r="D30">
-        <v>6.6E-3</v>
+        <v>-2.5200000000000001E-3</v>
       </c>
       <c r="E30">
-        <v>3.8</v>
+        <v>5</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1579,19 +1597,19 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31">
-        <v>0.11409999999999999</v>
+        <v>1.5100000000000001E-2</v>
       </c>
       <c r="C31">
-        <v>0.28420000000000001</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D31">
-        <v>-1.0500000000000001E-2</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="E31">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1608,19 +1626,19 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32">
-        <v>4.41E-2</v>
+        <v>-8.1600000000000006E-2</v>
       </c>
       <c r="C32">
-        <v>0.14829999999999999</v>
+        <v>4.9399999999999999E-2</v>
       </c>
       <c r="D32">
-        <v>-1.01E-3</v>
+        <v>6.6E-3</v>
       </c>
       <c r="E32">
-        <v>5</v>
+        <v>3.8</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1637,19 +1655,19 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33">
-        <v>3.9600000000000003E-2</v>
+        <v>0.11409999999999999</v>
       </c>
       <c r="C33">
-        <v>0.153</v>
+        <v>0.28420000000000001</v>
       </c>
       <c r="D33">
-        <v>-1.4400000000000001E-3</v>
+        <v>-1.0500000000000001E-2</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1666,16 +1684,16 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34">
-        <v>3.9699999999999999E-2</v>
+        <v>4.41E-2</v>
       </c>
       <c r="C34">
-        <v>0.13300000000000001</v>
+        <v>0.14829999999999999</v>
       </c>
       <c r="D34">
-        <v>-1.08E-3</v>
+        <v>-1.01E-3</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -1695,19 +1713,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35">
-        <v>-7.8899999999999998E-2</v>
+        <v>3.9600000000000003E-2</v>
       </c>
       <c r="C35">
-        <v>-1.72E-2</v>
+        <v>0.153</v>
       </c>
       <c r="D35">
-        <v>5.2900000000000004E-3</v>
+        <v>-1.4400000000000001E-3</v>
       </c>
       <c r="E35">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1724,19 +1742,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B36">
-        <v>0.13059999999999999</v>
+        <v>3.9699999999999999E-2</v>
       </c>
       <c r="C36">
-        <v>0.25700000000000001</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="D36">
-        <v>-4.3E-3</v>
+        <v>-1.08E-3</v>
       </c>
       <c r="E36">
-        <v>3.2</v>
+        <v>5</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1753,16 +1771,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="B37">
-        <v>0.03</v>
+        <v>2.69E-2</v>
       </c>
       <c r="C37">
-        <v>5.5800000000000002E-2</v>
+        <v>-0.15529999999999999</v>
       </c>
       <c r="D37">
-        <v>3.8000000000000002E-4</v>
+        <v>-3.6600000000000001E-3</v>
       </c>
       <c r="E37">
         <v>5</v>
@@ -1782,19 +1800,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B38">
-        <v>2.7900000000000001E-2</v>
+        <v>-7.8899999999999998E-2</v>
       </c>
       <c r="C38">
-        <v>1.3899999999999999E-2</v>
+        <v>-1.72E-2</v>
       </c>
       <c r="D38">
-        <v>4.0000000000000003E-5</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1811,19 +1829,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B39">
-        <v>2.4400000000000002E-2</v>
+        <v>0.13059999999999999</v>
       </c>
       <c r="C39">
-        <v>2.6200000000000001E-2</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="D39">
-        <v>-3.65E-3</v>
+        <v>-4.3E-3</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -1840,19 +1858,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40">
-        <v>4.2700000000000002E-2</v>
+        <v>0.03</v>
       </c>
       <c r="C40">
-        <v>0.06</v>
+        <v>5.5800000000000002E-2</v>
       </c>
       <c r="D40">
-        <v>-5.1000000000000004E-3</v>
+        <v>3.8000000000000002E-4</v>
       </c>
       <c r="E40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1869,19 +1887,19 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41">
-        <v>-8.5599999999999996E-2</v>
+        <v>2.7900000000000001E-2</v>
       </c>
       <c r="C41">
-        <v>2.5000000000000001E-3</v>
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="D41">
-        <v>5.9100000000000003E-3</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="E41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1898,19 +1916,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B42">
-        <v>5.2200000000000003E-2</v>
+        <v>2.4400000000000002E-2</v>
       </c>
       <c r="C42">
-        <v>0.1918</v>
+        <v>2.6200000000000001E-2</v>
       </c>
       <c r="D42">
-        <v>-3.0100000000000001E-3</v>
+        <v>-3.65E-3</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1927,19 +1945,19 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43">
-        <v>6.2399999999999997E-2</v>
+        <v>4.2700000000000002E-2</v>
       </c>
       <c r="C43">
-        <v>0.19470000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="D43">
-        <v>-4.3600000000000002E-3</v>
+        <v>-5.1000000000000004E-3</v>
       </c>
       <c r="E43">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -1956,16 +1974,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B44">
-        <v>-1.54E-2</v>
+        <v>-8.5599999999999996E-2</v>
       </c>
       <c r="C44">
-        <v>0.112</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D44">
-        <v>-3.0000000000000001E-5</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -1985,19 +2003,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B45">
-        <v>0.1124</v>
+        <v>5.2200000000000003E-2</v>
       </c>
       <c r="C45">
-        <v>0.24829999999999999</v>
+        <v>0.1918</v>
       </c>
       <c r="D45">
-        <v>-5.2500000000000003E-3</v>
+        <v>-3.0100000000000001E-3</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2014,19 +2032,19 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B46">
-        <v>8.2000000000000003E-2</v>
+        <v>6.2399999999999997E-2</v>
       </c>
       <c r="C46">
-        <v>0.28720000000000001</v>
+        <v>0.19470000000000001</v>
       </c>
       <c r="D46">
-        <v>-5.2300000000000003E-3</v>
+        <v>-4.3600000000000002E-3</v>
       </c>
       <c r="E46">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2043,19 +2061,19 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B47">
-        <v>0.1426</v>
+        <v>-1.54E-2</v>
       </c>
       <c r="C47">
-        <v>0.32369999999999999</v>
+        <v>0.112</v>
       </c>
       <c r="D47">
-        <v>-6.2899999999999996E-3</v>
+        <v>-3.0000000000000001E-5</v>
       </c>
       <c r="E47">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2072,19 +2090,19 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B48">
-        <v>0.1875</v>
+        <v>0.1124</v>
       </c>
       <c r="C48">
-        <v>0.27889999999999998</v>
+        <v>0.24829999999999999</v>
       </c>
       <c r="D48">
-        <v>-1.277E-2</v>
+        <v>-5.2500000000000003E-3</v>
       </c>
       <c r="E48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -2101,19 +2119,19 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B49">
-        <v>2.29E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C49">
-        <v>0.16</v>
+        <v>0.28720000000000001</v>
       </c>
       <c r="D49">
-        <v>-1.06E-3</v>
+        <v>-5.2300000000000003E-3</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -2130,19 +2148,19 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B50">
-        <v>3.5400000000000001E-2</v>
+        <v>0.1426</v>
       </c>
       <c r="C50">
-        <v>0.16059999999999999</v>
+        <v>0.32369999999999999</v>
       </c>
       <c r="D50">
-        <v>4.0000000000000002E-4</v>
+        <v>-6.2899999999999996E-3</v>
       </c>
       <c r="E50">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -2159,19 +2177,19 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B51">
-        <v>0.15870000000000001</v>
+        <v>0.1875</v>
       </c>
       <c r="C51">
-        <v>0.3251</v>
+        <v>0.27889999999999998</v>
       </c>
       <c r="D51">
-        <v>-6.6E-3</v>
+        <v>-1.277E-2</v>
       </c>
       <c r="E51">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -2188,16 +2206,16 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B52">
-        <v>-9.4999999999999998E-3</v>
+        <v>2.29E-2</v>
       </c>
       <c r="C52">
-        <v>0.14230000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="D52">
-        <v>1.67E-3</v>
+        <v>-1.06E-3</v>
       </c>
       <c r="E52">
         <v>5</v>
@@ -2217,19 +2235,19 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B53">
-        <v>1.11E-2</v>
+        <v>3.5400000000000001E-2</v>
       </c>
       <c r="C53">
-        <v>0.15640000000000001</v>
+        <v>0.16059999999999999</v>
       </c>
       <c r="D53">
-        <v>2.7399999999999998E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="E53">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2246,16 +2264,16 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B54">
-        <v>0.16220000000000001</v>
+        <v>0.15870000000000001</v>
       </c>
       <c r="C54">
-        <v>0.33529999999999999</v>
+        <v>0.3251</v>
       </c>
       <c r="D54">
-        <v>-5.5100000000000001E-3</v>
+        <v>-6.6E-3</v>
       </c>
       <c r="E54">
         <v>3.5</v>
@@ -2275,19 +2293,19 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B55">
-        <v>0.1628</v>
+        <v>-9.4999999999999998E-3</v>
       </c>
       <c r="C55">
-        <v>0.36049999999999999</v>
+        <v>0.14230000000000001</v>
       </c>
       <c r="D55">
-        <v>-5.5500000000000002E-3</v>
+        <v>1.67E-3</v>
       </c>
       <c r="E55">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2304,19 +2322,19 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B56">
-        <v>8.2000000000000007E-3</v>
+        <v>1.11E-2</v>
       </c>
       <c r="C56">
-        <v>1.3100000000000001E-2</v>
+        <v>0.15640000000000001</v>
       </c>
       <c r="D56">
-        <v>-1.2700000000000001E-3</v>
+        <v>2.7399999999999998E-3</v>
       </c>
       <c r="E56">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -2333,19 +2351,19 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B57">
-        <v>0.26769999999999999</v>
+        <v>0.16220000000000001</v>
       </c>
       <c r="C57">
-        <v>0.22650000000000001</v>
+        <v>0.33529999999999999</v>
       </c>
       <c r="D57">
-        <v>1.2999999999999999E-3</v>
+        <v>-5.5100000000000001E-3</v>
       </c>
       <c r="E57">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -2362,19 +2380,19 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B58">
-        <v>0.31130000000000002</v>
+        <v>0.1628</v>
       </c>
       <c r="C58">
-        <v>0.61550000000000005</v>
+        <v>0.36049999999999999</v>
       </c>
       <c r="D58">
-        <v>3.49E-2</v>
+        <v>-5.5500000000000002E-3</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2391,19 +2409,19 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B59">
-        <v>0.60919999999999996</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="C59">
-        <v>0.40200000000000002</v>
+        <v>1.3100000000000001E-2</v>
       </c>
       <c r="D59">
-        <v>-2.81E-2</v>
+        <v>-1.2700000000000001E-3</v>
       </c>
       <c r="E59">
-        <v>1.7</v>
+        <v>6</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -2420,19 +2438,19 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B60">
-        <v>1.49E-2</v>
+        <v>0.26769999999999999</v>
       </c>
       <c r="C60">
-        <v>-8.3000000000000004E-2</v>
+        <v>0.22650000000000001</v>
       </c>
       <c r="D60">
-        <v>5.7000000000000002E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="E60">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2449,19 +2467,19 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B61">
-        <v>3.3599999999999998E-2</v>
+        <v>0.31130000000000002</v>
       </c>
       <c r="C61">
-        <v>-0.153</v>
+        <v>0.61550000000000005</v>
       </c>
       <c r="D61">
-        <v>8.3999999999999995E-3</v>
+        <v>3.49E-2</v>
       </c>
       <c r="E61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2478,19 +2496,19 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B62">
-        <v>0.1065</v>
+        <v>0.60919999999999996</v>
       </c>
       <c r="C62">
-        <v>-0.35399999999999998</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="D62">
-        <v>9.7999999999999997E-3</v>
+        <v>-2.81E-2</v>
       </c>
       <c r="E62">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2507,19 +2525,19 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B63">
-        <v>0.20580000000000001</v>
+        <v>1.49E-2</v>
       </c>
       <c r="C63">
-        <v>-0.46400000000000002</v>
+        <v>-8.3000000000000004E-2</v>
       </c>
       <c r="D63">
-        <v>-5.8799999999999998E-2</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="E63">
-        <v>2.5</v>
+        <v>3.4</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2536,19 +2554,19 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B64">
-        <v>-3.6299999999999999E-2</v>
+        <v>3.3599999999999998E-2</v>
       </c>
       <c r="C64">
-        <v>-0.20100000000000001</v>
+        <v>-0.153</v>
       </c>
       <c r="D64">
         <v>8.3999999999999995E-3</v>
       </c>
       <c r="E64">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2565,19 +2583,19 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B65">
-        <v>-4.5699999999999998E-2</v>
+        <v>0.1065</v>
       </c>
       <c r="C65">
-        <v>-0.44800000000000001</v>
+        <v>-0.35399999999999998</v>
       </c>
       <c r="D65">
-        <v>1.35E-2</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2594,19 +2612,19 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B66">
-        <v>1.0800000000000001E-2</v>
+        <v>0.20580000000000001</v>
       </c>
       <c r="C66">
-        <v>-0.82599999999999996</v>
+        <v>-0.46400000000000002</v>
       </c>
       <c r="D66">
-        <v>7.7999999999999996E-3</v>
+        <v>-5.8799999999999998E-2</v>
       </c>
       <c r="E66">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2623,19 +2641,19 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B67">
-        <v>-5.5800000000000002E-2</v>
+        <v>-3.6299999999999999E-2</v>
       </c>
       <c r="C67">
-        <v>-0.57899999999999996</v>
+        <v>-0.20100000000000001</v>
       </c>
       <c r="D67">
-        <v>-1E-3</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="E67">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2652,19 +2670,19 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B68">
-        <v>-0.193</v>
+        <v>-4.5699999999999998E-2</v>
       </c>
       <c r="C68">
-        <v>-0.59899999999999998</v>
+        <v>-0.44800000000000001</v>
       </c>
       <c r="D68">
-        <v>4.0099999999999997E-2</v>
+        <v>1.35E-2</v>
       </c>
       <c r="E68">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2681,19 +2699,19 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B69">
-        <v>0.1298</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="C69">
-        <v>0.629</v>
+        <v>-0.82599999999999996</v>
       </c>
       <c r="D69">
-        <v>5.1999999999999998E-3</v>
+        <v>7.7999999999999996E-3</v>
       </c>
       <c r="E69">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -2710,19 +2728,19 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B70">
-        <v>0.13200000000000001</v>
+        <v>-5.5800000000000002E-2</v>
       </c>
       <c r="C70">
-        <v>0.27100000000000002</v>
+        <v>-0.57899999999999996</v>
       </c>
       <c r="D70">
-        <v>-3.0000000000000001E-3</v>
+        <v>-1E-3</v>
       </c>
       <c r="E70">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2739,19 +2757,19 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B71">
-        <v>0.78700000000000003</v>
+        <v>-0.193</v>
       </c>
       <c r="C71">
-        <v>0.27400000000000002</v>
+        <v>-0.59899999999999998</v>
       </c>
       <c r="D71">
-        <v>-2.3999999999999998E-3</v>
+        <v>4.0099999999999997E-2</v>
       </c>
       <c r="E71">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2768,16 +2786,16 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B72">
-        <v>5.8099999999999999E-2</v>
+        <v>0.1298</v>
       </c>
       <c r="C72">
-        <v>0.16500000000000001</v>
+        <v>0.629</v>
       </c>
       <c r="D72">
-        <v>-4.5999999999999999E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="E72">
         <v>4</v>
@@ -2797,16 +2815,16 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B73">
-        <v>6.6100000000000006E-2</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="C73">
-        <v>0.191</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="D73">
-        <v>-4.1000000000000003E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="E73">
         <v>4</v>
@@ -2826,16 +2844,16 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B74">
-        <v>0.14580000000000001</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="C74">
-        <v>0.16800000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="D74">
-        <v>-4.3E-3</v>
+        <v>-2.3999999999999998E-3</v>
       </c>
       <c r="E74">
         <v>4</v>
@@ -2855,16 +2873,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B75">
-        <v>0.15479999999999999</v>
+        <v>5.8099999999999999E-2</v>
       </c>
       <c r="C75">
-        <v>0.09</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D75">
-        <v>-3.3999999999999998E-3</v>
+        <v>-4.5999999999999999E-3</v>
       </c>
       <c r="E75">
         <v>4</v>
@@ -2884,16 +2902,16 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B76">
-        <v>0.2145</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="C76">
-        <v>0.23499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="D76">
-        <v>-3.9199999999999999E-2</v>
+        <v>-4.1000000000000003E-3</v>
       </c>
       <c r="E76">
         <v>4</v>
@@ -2913,16 +2931,16 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B77">
-        <v>0.15359999999999999</v>
+        <v>0.14580000000000001</v>
       </c>
       <c r="C77">
-        <v>0.34100000000000003</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="D77">
-        <v>-5.5999999999999999E-3</v>
+        <v>-4.3E-3</v>
       </c>
       <c r="E77">
         <v>4</v>
@@ -2942,16 +2960,16 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B78">
-        <v>0.1799</v>
+        <v>0.15479999999999999</v>
       </c>
       <c r="C78">
-        <v>0.31900000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="D78">
-        <v>-1.18E-2</v>
+        <v>-3.3999999999999998E-3</v>
       </c>
       <c r="E78">
         <v>4</v>
@@ -2971,16 +2989,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B79">
-        <v>0.13159999999999999</v>
+        <v>0.2145</v>
       </c>
       <c r="C79">
-        <v>0.374</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="D79">
-        <v>-8.2000000000000007E-3</v>
+        <v>-3.9199999999999999E-2</v>
       </c>
       <c r="E79">
         <v>4</v>
@@ -3000,16 +3018,16 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B80">
-        <v>9.6500000000000002E-2</v>
+        <v>0.15359999999999999</v>
       </c>
       <c r="C80">
-        <v>0.25</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="D80">
-        <v>-7.4000000000000003E-3</v>
+        <v>-5.5999999999999999E-3</v>
       </c>
       <c r="E80">
         <v>4</v>
@@ -3029,16 +3047,16 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B81">
-        <v>0.1142</v>
+        <v>0.1799</v>
       </c>
       <c r="C81">
-        <v>0.17899999999999999</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="D81">
-        <v>-1.14E-2</v>
+        <v>-1.18E-2</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -3058,16 +3076,16 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B82">
-        <v>0.1792</v>
+        <v>0.13159999999999999</v>
       </c>
       <c r="C82">
-        <v>8.3000000000000004E-2</v>
+        <v>0.374</v>
       </c>
       <c r="D82">
-        <v>-1.1599999999999999E-2</v>
+        <v>-8.2000000000000007E-3</v>
       </c>
       <c r="E82">
         <v>4</v>
@@ -3087,16 +3105,16 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B83">
-        <v>0.18049999999999999</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="C83">
-        <v>7.4999999999999997E-2</v>
+        <v>0.25</v>
       </c>
       <c r="D83">
-        <v>-4.0000000000000001E-3</v>
+        <v>-7.4000000000000003E-3</v>
       </c>
       <c r="E83">
         <v>4</v>
@@ -3116,16 +3134,16 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B84">
-        <v>0.1827</v>
+        <v>0.1142</v>
       </c>
       <c r="C84">
-        <v>0.44500000000000001</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="D84">
-        <v>3.5999999999999999E-3</v>
+        <v>-1.14E-2</v>
       </c>
       <c r="E84">
         <v>4</v>
@@ -3145,19 +3163,19 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B85">
-        <v>5.2600000000000001E-2</v>
+        <v>0.1792</v>
       </c>
       <c r="C85">
-        <v>0.44500000000000001</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D85">
-        <v>3.5999999999999999E-3</v>
+        <v>-1.1599999999999999E-2</v>
       </c>
       <c r="E85">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -3174,19 +3192,19 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B86">
-        <v>0.1134</v>
+        <v>0.18049999999999999</v>
       </c>
       <c r="C86">
-        <v>0.46600000000000003</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="D86">
-        <v>-7.4999999999999997E-3</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="E86">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -3203,19 +3221,19 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B87">
-        <v>8.4199999999999997E-2</v>
+        <v>0.1827</v>
       </c>
       <c r="C87">
-        <v>0.35099999999999998</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="D87">
-        <v>-1.8100000000000002E-2</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E87">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -3232,19 +3250,19 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B88">
-        <v>1.89E-2</v>
+        <v>5.2600000000000001E-2</v>
       </c>
       <c r="C88">
-        <v>0.39900000000000002</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="D88">
-        <v>4.5999999999999999E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E88">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -3261,19 +3279,19 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B89">
-        <v>-3.44E-2</v>
+        <v>0.1134</v>
       </c>
       <c r="C89">
-        <v>0.39600000000000002</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="D89">
-        <v>4.3E-3</v>
+        <v>-7.4999999999999997E-3</v>
       </c>
       <c r="E89">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -3290,19 +3308,19 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B90">
-        <v>-9.8500000000000004E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
       <c r="C90">
-        <v>0.45300000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="D90">
-        <v>1.2200000000000001E-2</v>
+        <v>-1.8100000000000002E-2</v>
       </c>
       <c r="E90">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -3319,16 +3337,16 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B91">
-        <v>-9.6500000000000002E-2</v>
+        <v>1.89E-2</v>
       </c>
       <c r="C91">
-        <v>0.14099999999999999</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="D91">
-        <v>2.1000000000000001E-2</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="E91">
         <v>4.5</v>
@@ -3348,19 +3366,19 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B92">
-        <v>-9.7999999999999997E-3</v>
+        <v>-3.44E-2</v>
       </c>
       <c r="C92">
-        <v>0.36099999999999999</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="D92">
-        <v>3.8999999999999998E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="E92">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -3377,19 +3395,19 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B93">
-        <v>-0.1736</v>
+        <v>-9.8500000000000004E-2</v>
       </c>
       <c r="C93">
-        <v>0.435</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="D93">
-        <v>3.8300000000000001E-2</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="E93">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -3406,19 +3424,19 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B94">
-        <v>-0.14380000000000001</v>
+        <v>-9.6500000000000002E-2</v>
       </c>
       <c r="C94">
-        <v>0.80400000000000005</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D94">
-        <v>3.1699999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="E94">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -3435,19 +3453,19 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B95">
-        <v>-0.224</v>
+        <v>-9.7999999999999997E-3</v>
       </c>
       <c r="C95">
-        <v>0.89500000000000002</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="D95">
-        <v>3.5499999999999997E-2</v>
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="E95">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -3464,16 +3482,16 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B96">
-        <v>-0.22090000000000001</v>
+        <v>-0.1736</v>
       </c>
       <c r="C96">
-        <v>0.248</v>
+        <v>0.435</v>
       </c>
       <c r="D96">
-        <v>4.3200000000000002E-2</v>
+        <v>3.8300000000000001E-2</v>
       </c>
       <c r="E96">
         <v>2</v>
@@ -3493,19 +3511,19 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B97">
-        <v>-0.1198</v>
+        <v>-0.14380000000000001</v>
       </c>
       <c r="C97">
-        <v>0.871</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="D97">
-        <v>4.5620000000000001E-2</v>
+        <v>3.1699999999999999E-2</v>
       </c>
       <c r="E97">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -3522,19 +3540,19 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B98">
-        <v>4.5699999999999998E-2</v>
+        <v>-0.224</v>
       </c>
       <c r="C98">
-        <v>-0.19600000000000001</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="D98">
-        <v>8.0000000000000004E-4</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="E98">
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -3551,19 +3569,19 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B99">
-        <v>-6.6E-3</v>
+        <v>-0.22090000000000001</v>
       </c>
       <c r="C99">
-        <v>-0.22700000000000001</v>
+        <v>0.248</v>
       </c>
       <c r="D99">
-        <v>3.5999999999999999E-3</v>
+        <v>4.3200000000000002E-2</v>
       </c>
       <c r="E99">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -3580,19 +3598,19 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B100">
-        <v>-8.2100000000000006E-2</v>
+        <v>-0.1198</v>
       </c>
       <c r="C100">
-        <v>-0.17799999999999999</v>
+        <v>0.871</v>
       </c>
       <c r="D100">
-        <v>1.6199999999999999E-2</v>
+        <v>4.5620000000000001E-2</v>
       </c>
       <c r="E100">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -3609,19 +3627,19 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B101">
-        <v>-0.1517</v>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="C101">
-        <v>-0.54500000000000004</v>
+        <v>-0.19600000000000001</v>
       </c>
       <c r="D101">
-        <v>1.8700000000000001E-2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E101">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -3638,19 +3656,19 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B102">
-        <v>-8.7900000000000006E-2</v>
+        <v>-6.6E-3</v>
       </c>
       <c r="C102">
-        <v>-0.34300000000000003</v>
+        <v>-0.22700000000000001</v>
       </c>
       <c r="D102">
-        <v>1.34E-2</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E102">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -3667,19 +3685,19 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B103">
-        <v>-0.15179999999999999</v>
+        <v>-8.2100000000000006E-2</v>
       </c>
       <c r="C103">
-        <v>-0.77800000000000002</v>
+        <v>-0.17799999999999999</v>
       </c>
       <c r="D103">
-        <v>1.77E-2</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="E103">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -3696,19 +3714,19 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B104">
-        <v>9.3799999999999994E-2</v>
+        <v>-0.1517</v>
       </c>
       <c r="C104">
-        <v>0.128</v>
+        <v>-0.54500000000000004</v>
       </c>
       <c r="D104">
-        <v>-3.0000000000000001E-3</v>
+        <v>1.8700000000000001E-2</v>
       </c>
       <c r="E104">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3725,19 +3743,19 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B105">
-        <v>-4.7399999999999998E-2</v>
+        <v>-8.7900000000000006E-2</v>
       </c>
       <c r="C105">
-        <v>-0.25900000000000001</v>
+        <v>-0.34300000000000003</v>
       </c>
       <c r="D105">
-        <v>1.06E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="E105">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3754,19 +3772,19 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B106">
-        <v>3.1399999999999997E-2</v>
+        <v>-0.15179999999999999</v>
       </c>
       <c r="C106">
-        <v>-0.184</v>
+        <v>-0.77800000000000002</v>
       </c>
       <c r="D106">
-        <v>2.3E-3</v>
+        <v>1.77E-2</v>
       </c>
       <c r="E106">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3783,19 +3801,19 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B107">
-        <v>-2.2800000000000001E-2</v>
+        <v>9.3799999999999994E-2</v>
       </c>
       <c r="C107">
-        <v>-0.245</v>
+        <v>0.128</v>
       </c>
       <c r="D107">
-        <v>4.4000000000000003E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="E107">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -3812,16 +3830,16 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B108">
-        <v>-0.60099999999999998</v>
+        <v>-4.7399999999999998E-2</v>
       </c>
       <c r="C108">
-        <v>-0.60399999999999998</v>
+        <v>-0.25900000000000001</v>
       </c>
       <c r="D108">
-        <v>6.0000000000000001E-3</v>
+        <v>1.06E-2</v>
       </c>
       <c r="E108">
         <v>3</v>
@@ -3841,16 +3859,16 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B109">
-        <v>7.2599999999999998E-2</v>
+        <v>3.1399999999999997E-2</v>
       </c>
       <c r="C109">
-        <v>-0.245</v>
+        <v>-0.184</v>
       </c>
       <c r="D109">
-        <v>-9.9000000000000008E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="E109">
         <v>6</v>
@@ -3870,16 +3888,16 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B110">
-        <v>-8.0299999999999996E-2</v>
+        <v>-2.2800000000000001E-2</v>
       </c>
       <c r="C110">
-        <v>-0.61599999999999999</v>
+        <v>-0.245</v>
       </c>
       <c r="D110">
-        <v>5.3E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="E110">
         <v>6</v>
@@ -3894,6 +3912,93 @@
         <v>1</v>
       </c>
       <c r="I110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111">
+        <v>-0.60099999999999998</v>
+      </c>
+      <c r="C111">
+        <v>-0.60399999999999998</v>
+      </c>
+      <c r="D111">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E111">
+        <v>3</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
+      </c>
+      <c r="G111">
+        <v>-1</v>
+      </c>
+      <c r="H111">
+        <v>1</v>
+      </c>
+      <c r="I111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>107</v>
+      </c>
+      <c r="B112">
+        <v>7.2599999999999998E-2</v>
+      </c>
+      <c r="C112">
+        <v>-0.245</v>
+      </c>
+      <c r="D112">
+        <v>-9.9000000000000008E-3</v>
+      </c>
+      <c r="E112">
+        <v>6</v>
+      </c>
+      <c r="F112">
+        <v>1</v>
+      </c>
+      <c r="G112">
+        <v>-1</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
+      <c r="I112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>108</v>
+      </c>
+      <c r="B113">
+        <v>-8.0299999999999996E-2</v>
+      </c>
+      <c r="C113">
+        <v>-0.61599999999999999</v>
+      </c>
+      <c r="D113">
+        <v>5.3E-3</v>
+      </c>
+      <c r="E113">
+        <v>6</v>
+      </c>
+      <c r="F113">
+        <v>1</v>
+      </c>
+      <c r="G113">
+        <v>-1</v>
+      </c>
+      <c r="H113">
+        <v>1</v>
+      </c>
+      <c r="I113">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected a few typos in the data file
</commit_message>
<xml_diff>
--- a/aqpolypy/salt/paramsPM.xlsx
+++ b/aqpolypy/salt/paramsPM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trvsst\Research\aqpolypy\aqpolypy\salt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13372E3C-1097-4905-A855-2C42049CB257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFFC7F0-E012-401A-AD14-2CCD20D8DE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>HCl</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>RbNO2</t>
+  </si>
+  <si>
+    <t>Pr4NF</t>
   </si>
 </sst>
 </file>
@@ -714,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2496,19 +2499,19 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="B62">
-        <v>0.60919999999999996</v>
+        <v>0.44629999999999997</v>
       </c>
       <c r="C62">
-        <v>0.40200000000000002</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="D62">
-        <v>-2.81E-2</v>
+        <v>5.3699999999999998E-2</v>
       </c>
       <c r="E62">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2525,19 +2528,19 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63">
-        <v>1.49E-2</v>
+        <v>0.60919999999999996</v>
       </c>
       <c r="C63">
-        <v>-8.3000000000000004E-2</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="D63">
-        <v>5.7000000000000002E-3</v>
+        <v>-2.81E-2</v>
       </c>
       <c r="E63">
-        <v>3.4</v>
+        <v>1.7</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2554,19 +2557,19 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64">
-        <v>3.3599999999999998E-2</v>
+        <v>1.49E-2</v>
       </c>
       <c r="C64">
-        <v>-0.153</v>
+        <v>-8.3000000000000004E-2</v>
       </c>
       <c r="D64">
-        <v>8.3999999999999995E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="E64">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2583,19 +2586,19 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65">
-        <v>0.1065</v>
+        <v>3.3599999999999998E-2</v>
       </c>
       <c r="C65">
-        <v>-0.35399999999999998</v>
+        <v>-0.153</v>
       </c>
       <c r="D65">
-        <v>9.7999999999999997E-3</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="E65">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2612,16 +2615,16 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66">
-        <v>0.20580000000000001</v>
+        <v>0.1065</v>
       </c>
       <c r="C66">
-        <v>-0.46400000000000002</v>
+        <v>-0.35399999999999998</v>
       </c>
       <c r="D66">
-        <v>-5.8799999999999998E-2</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="E66">
         <v>2.5</v>
@@ -2641,19 +2644,19 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B67">
-        <v>-3.6299999999999999E-2</v>
+        <v>0.20580000000000001</v>
       </c>
       <c r="C67">
-        <v>-0.20100000000000001</v>
+        <v>-0.46400000000000002</v>
       </c>
       <c r="D67">
-        <v>8.3999999999999995E-3</v>
+        <v>-5.8799999999999998E-2</v>
       </c>
       <c r="E67">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2670,19 +2673,19 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68">
-        <v>-4.5699999999999998E-2</v>
+        <v>-3.6299999999999999E-2</v>
       </c>
       <c r="C68">
-        <v>-0.44800000000000001</v>
+        <v>-0.20100000000000001</v>
       </c>
       <c r="D68">
-        <v>1.35E-2</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="E68">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2699,19 +2702,19 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69">
-        <v>1.0800000000000001E-2</v>
+        <v>-4.5699999999999998E-2</v>
       </c>
       <c r="C69">
-        <v>-0.82599999999999996</v>
+        <v>-0.44800000000000001</v>
       </c>
       <c r="D69">
-        <v>7.7999999999999996E-3</v>
+        <v>1.35E-2</v>
       </c>
       <c r="E69">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -2728,19 +2731,19 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B70">
-        <v>-5.5800000000000002E-2</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="C70">
-        <v>-0.57899999999999996</v>
+        <v>-0.82599999999999996</v>
       </c>
       <c r="D70">
-        <v>-1E-3</v>
+        <v>7.7999999999999996E-3</v>
       </c>
       <c r="E70">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2757,19 +2760,19 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71">
-        <v>-0.193</v>
+        <v>-5.5800000000000002E-2</v>
       </c>
       <c r="C71">
-        <v>-0.59899999999999998</v>
+        <v>-0.57899999999999996</v>
       </c>
       <c r="D71">
-        <v>4.0099999999999997E-2</v>
+        <v>-1E-3</v>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2786,19 +2789,19 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B72">
-        <v>0.1298</v>
+        <v>-0.193</v>
       </c>
       <c r="C72">
-        <v>0.629</v>
+        <v>-0.59899999999999998</v>
       </c>
       <c r="D72">
-        <v>5.1999999999999998E-3</v>
+        <v>4.0099999999999997E-2</v>
       </c>
       <c r="E72">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2815,16 +2818,16 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B73">
-        <v>0.13200000000000001</v>
+        <v>0.1298</v>
       </c>
       <c r="C73">
-        <v>0.27100000000000002</v>
+        <v>0.629</v>
       </c>
       <c r="D73">
-        <v>-3.0000000000000001E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="E73">
         <v>4</v>
@@ -2844,16 +2847,16 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B74">
-        <v>0.78700000000000003</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="C74">
-        <v>0.27400000000000002</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="D74">
-        <v>-2.3999999999999998E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="E74">
         <v>4</v>
@@ -2873,16 +2876,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B75">
-        <v>5.8099999999999999E-2</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="C75">
-        <v>0.16500000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="D75">
-        <v>-4.5999999999999999E-3</v>
+        <v>-2.3999999999999998E-3</v>
       </c>
       <c r="E75">
         <v>4</v>
@@ -2902,16 +2905,16 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B76">
-        <v>6.6100000000000006E-2</v>
+        <v>5.8099999999999999E-2</v>
       </c>
       <c r="C76">
-        <v>0.191</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D76">
-        <v>-4.1000000000000003E-3</v>
+        <v>-4.5999999999999999E-3</v>
       </c>
       <c r="E76">
         <v>4</v>
@@ -2931,16 +2934,16 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B77">
-        <v>0.14580000000000001</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="C77">
-        <v>0.16800000000000001</v>
+        <v>0.191</v>
       </c>
       <c r="D77">
-        <v>-4.3E-3</v>
+        <v>-4.1000000000000003E-3</v>
       </c>
       <c r="E77">
         <v>4</v>
@@ -2960,16 +2963,16 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B78">
-        <v>0.15479999999999999</v>
+        <v>0.14580000000000001</v>
       </c>
       <c r="C78">
-        <v>0.09</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="D78">
-        <v>-3.3999999999999998E-3</v>
+        <v>-4.3E-3</v>
       </c>
       <c r="E78">
         <v>4</v>
@@ -2989,16 +2992,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B79">
-        <v>0.2145</v>
+        <v>0.15479999999999999</v>
       </c>
       <c r="C79">
-        <v>0.23499999999999999</v>
+        <v>0.09</v>
       </c>
       <c r="D79">
-        <v>-3.9199999999999999E-2</v>
+        <v>-3.3999999999999998E-3</v>
       </c>
       <c r="E79">
         <v>4</v>
@@ -3018,16 +3021,16 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B80">
-        <v>0.15359999999999999</v>
+        <v>0.2145</v>
       </c>
       <c r="C80">
-        <v>0.34100000000000003</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="D80">
-        <v>-5.5999999999999999E-3</v>
+        <v>-3.9199999999999999E-2</v>
       </c>
       <c r="E80">
         <v>4</v>
@@ -3047,16 +3050,16 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B81">
-        <v>0.1799</v>
+        <v>0.15359999999999999</v>
       </c>
       <c r="C81">
-        <v>0.31900000000000001</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="D81">
-        <v>-1.18E-2</v>
+        <v>-5.5999999999999999E-3</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -3076,16 +3079,16 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B82">
-        <v>0.13159999999999999</v>
+        <v>0.1799</v>
       </c>
       <c r="C82">
-        <v>0.374</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="D82">
-        <v>-8.2000000000000007E-3</v>
+        <v>-1.18E-2</v>
       </c>
       <c r="E82">
         <v>4</v>
@@ -3105,16 +3108,16 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B83">
-        <v>9.6500000000000002E-2</v>
+        <v>0.13159999999999999</v>
       </c>
       <c r="C83">
-        <v>0.25</v>
+        <v>0.374</v>
       </c>
       <c r="D83">
-        <v>-7.4000000000000003E-3</v>
+        <v>-8.2000000000000007E-3</v>
       </c>
       <c r="E83">
         <v>4</v>
@@ -3134,16 +3137,16 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84">
-        <v>0.1142</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="C84">
-        <v>0.17899999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="D84">
-        <v>-1.14E-2</v>
+        <v>-7.4000000000000003E-3</v>
       </c>
       <c r="E84">
         <v>4</v>
@@ -3163,16 +3166,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B85">
-        <v>0.1792</v>
+        <v>0.1142</v>
       </c>
       <c r="C85">
-        <v>8.3000000000000004E-2</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="D85">
-        <v>-1.1599999999999999E-2</v>
+        <v>-1.14E-2</v>
       </c>
       <c r="E85">
         <v>4</v>
@@ -3192,16 +3195,16 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B86">
-        <v>0.18049999999999999</v>
+        <v>0.1792</v>
       </c>
       <c r="C86">
-        <v>7.4999999999999997E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D86">
-        <v>-4.0000000000000001E-3</v>
+        <v>-1.1599999999999999E-2</v>
       </c>
       <c r="E86">
         <v>4</v>
@@ -3221,16 +3224,16 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87">
-        <v>0.1827</v>
+        <v>0.18049999999999999</v>
       </c>
       <c r="C87">
-        <v>0.44500000000000001</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="D87">
-        <v>3.5999999999999999E-3</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="E87">
         <v>4</v>
@@ -3250,10 +3253,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B88">
-        <v>5.2600000000000001E-2</v>
+        <v>0.1827</v>
       </c>
       <c r="C88">
         <v>0.44500000000000001</v>
@@ -3262,7 +3265,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="E88">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -3279,19 +3282,19 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89">
-        <v>0.1134</v>
+        <v>5.2600000000000001E-2</v>
       </c>
       <c r="C89">
-        <v>0.46600000000000003</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="D89">
-        <v>-7.4999999999999997E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E89">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -3308,19 +3311,19 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90">
-        <v>8.4199999999999997E-2</v>
+        <v>0.1134</v>
       </c>
       <c r="C90">
-        <v>0.35099999999999998</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="D90">
-        <v>-1.8100000000000002E-2</v>
+        <v>-7.4999999999999997E-3</v>
       </c>
       <c r="E90">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -3337,19 +3340,19 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B91">
-        <v>1.89E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
       <c r="C91">
-        <v>0.39900000000000002</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="D91">
-        <v>4.5999999999999999E-3</v>
+        <v>-1.8100000000000002E-2</v>
       </c>
       <c r="E91">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -3366,19 +3369,19 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B92">
-        <v>-3.44E-2</v>
+        <v>1.89E-2</v>
       </c>
       <c r="C92">
-        <v>0.39600000000000002</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="D92">
-        <v>4.3E-3</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="E92">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -3395,19 +3398,19 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B93">
-        <v>-9.8500000000000004E-2</v>
+        <v>-3.44E-2</v>
       </c>
       <c r="C93">
-        <v>0.45300000000000001</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="D93">
-        <v>1.2200000000000001E-2</v>
+        <v>4.3E-3</v>
       </c>
       <c r="E93">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -3424,19 +3427,19 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B94">
-        <v>-9.6500000000000002E-2</v>
+        <v>-9.8500000000000004E-2</v>
       </c>
       <c r="C94">
-        <v>0.14099999999999999</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="D94">
-        <v>2.1000000000000001E-2</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="E94">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -3453,19 +3456,19 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B95">
-        <v>-9.7999999999999997E-3</v>
+        <v>-9.6500000000000002E-2</v>
       </c>
       <c r="C95">
-        <v>0.36099999999999999</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D95">
-        <v>3.8999999999999998E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="E95">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -3482,19 +3485,19 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B96">
-        <v>-0.1736</v>
+        <v>-9.7999999999999997E-3</v>
       </c>
       <c r="C96">
-        <v>0.435</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="D96">
-        <v>3.8300000000000001E-2</v>
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="E96">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -3511,19 +3514,19 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B97">
-        <v>-0.14380000000000001</v>
+        <v>-0.1736</v>
       </c>
       <c r="C97">
-        <v>0.80400000000000005</v>
+        <v>0.435</v>
       </c>
       <c r="D97">
-        <v>3.1699999999999999E-2</v>
+        <v>3.8300000000000001E-2</v>
       </c>
       <c r="E97">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -3540,19 +3543,19 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B98">
-        <v>-0.224</v>
+        <v>-0.14380000000000001</v>
       </c>
       <c r="C98">
-        <v>0.89500000000000002</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="D98">
-        <v>3.5499999999999997E-2</v>
+        <v>3.1699999999999999E-2</v>
       </c>
       <c r="E98">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -3569,19 +3572,19 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B99">
-        <v>-0.22090000000000001</v>
+        <v>-0.224</v>
       </c>
       <c r="C99">
-        <v>0.248</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="D99">
-        <v>4.3200000000000002E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="E99">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -3598,16 +3601,16 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B100">
-        <v>-0.1198</v>
+        <v>-0.22090000000000001</v>
       </c>
       <c r="C100">
-        <v>0.871</v>
+        <v>0.248</v>
       </c>
       <c r="D100">
-        <v>4.5620000000000001E-2</v>
+        <v>4.3200000000000002E-2</v>
       </c>
       <c r="E100">
         <v>2</v>
@@ -3627,19 +3630,19 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B101">
-        <v>4.5699999999999998E-2</v>
+        <v>-0.1198</v>
       </c>
       <c r="C101">
-        <v>-0.19600000000000001</v>
+        <v>0.871</v>
       </c>
       <c r="D101">
-        <v>8.0000000000000004E-4</v>
+        <v>4.5620000000000001E-2</v>
       </c>
       <c r="E101">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -3656,16 +3659,16 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B102">
-        <v>-6.6E-3</v>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="C102">
-        <v>-0.22700000000000001</v>
+        <v>-0.19600000000000001</v>
       </c>
       <c r="D102">
-        <v>3.5999999999999999E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E102">
         <v>6</v>
@@ -3685,19 +3688,19 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B103">
-        <v>-8.2100000000000006E-2</v>
+        <v>-6.6E-3</v>
       </c>
       <c r="C103">
-        <v>-0.17799999999999999</v>
+        <v>-0.22700000000000001</v>
       </c>
       <c r="D103">
-        <v>1.6199999999999999E-2</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E103">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -3714,19 +3717,19 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B104">
-        <v>-0.1517</v>
+        <v>-8.2100000000000006E-2</v>
       </c>
       <c r="C104">
-        <v>-0.54500000000000004</v>
+        <v>-0.17799999999999999</v>
       </c>
       <c r="D104">
-        <v>1.8700000000000001E-2</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="E104">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3743,19 +3746,19 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B105">
-        <v>-8.7900000000000006E-2</v>
+        <v>-0.1517</v>
       </c>
       <c r="C105">
-        <v>-0.34300000000000003</v>
+        <v>-0.54500000000000004</v>
       </c>
       <c r="D105">
-        <v>1.34E-2</v>
+        <v>1.8700000000000001E-2</v>
       </c>
       <c r="E105">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3772,19 +3775,19 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B106">
-        <v>-0.15179999999999999</v>
+        <v>-8.7900000000000006E-2</v>
       </c>
       <c r="C106">
-        <v>-0.77800000000000002</v>
+        <v>-0.34300000000000003</v>
       </c>
       <c r="D106">
-        <v>1.77E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="E106">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3801,19 +3804,19 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B107">
-        <v>9.3799999999999994E-2</v>
+        <v>-0.15179999999999999</v>
       </c>
       <c r="C107">
-        <v>0.128</v>
+        <v>-0.77800000000000002</v>
       </c>
       <c r="D107">
-        <v>-3.0000000000000001E-3</v>
+        <v>1.77E-2</v>
       </c>
       <c r="E107">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -3830,19 +3833,19 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B108">
-        <v>-4.7399999999999998E-2</v>
+        <v>9.3799999999999994E-2</v>
       </c>
       <c r="C108">
-        <v>-0.25900000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="D108">
-        <v>1.06E-2</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="E108">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -3859,19 +3862,19 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B109">
-        <v>3.1399999999999997E-2</v>
+        <v>-4.7399999999999998E-2</v>
       </c>
       <c r="C109">
-        <v>-0.184</v>
+        <v>-0.25900000000000001</v>
       </c>
       <c r="D109">
-        <v>2.3E-3</v>
+        <v>1.06E-2</v>
       </c>
       <c r="E109">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -3888,16 +3891,16 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B110">
-        <v>-2.2800000000000001E-2</v>
+        <v>3.1399999999999997E-2</v>
       </c>
       <c r="C110">
-        <v>-0.245</v>
+        <v>-0.184</v>
       </c>
       <c r="D110">
-        <v>4.4000000000000003E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="E110">
         <v>6</v>
@@ -3917,19 +3920,19 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B111">
-        <v>-0.60099999999999998</v>
+        <v>-2.2800000000000001E-2</v>
       </c>
       <c r="C111">
-        <v>-0.60399999999999998</v>
+        <v>-0.245</v>
       </c>
       <c r="D111">
-        <v>6.0000000000000001E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="E111">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -3946,19 +3949,19 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B112">
-        <v>7.2599999999999998E-2</v>
+        <v>-0.60099999999999998</v>
       </c>
       <c r="C112">
-        <v>-0.245</v>
+        <v>-0.60399999999999998</v>
       </c>
       <c r="D112">
-        <v>-9.9000000000000008E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E112">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -3975,16 +3978,16 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B113">
-        <v>-8.0299999999999996E-2</v>
+        <v>7.2599999999999998E-2</v>
       </c>
       <c r="C113">
-        <v>-0.61599999999999999</v>
+        <v>-0.245</v>
       </c>
       <c r="D113">
-        <v>5.3E-3</v>
+        <v>-9.9000000000000008E-3</v>
       </c>
       <c r="E113">
         <v>6</v>
@@ -3999,6 +4002,35 @@
         <v>1</v>
       </c>
       <c r="I113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>108</v>
+      </c>
+      <c r="B114">
+        <v>-8.0299999999999996E-2</v>
+      </c>
+      <c r="C114">
+        <v>-0.61599999999999999</v>
+      </c>
+      <c r="D114">
+        <v>5.3E-3</v>
+      </c>
+      <c r="E114">
+        <v>6</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="G114">
+        <v>-1</v>
+      </c>
+      <c r="H114">
+        <v>1</v>
+      </c>
+      <c r="I114">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrections to salt param
</commit_message>
<xml_diff>
--- a/aqpolypy/salt/paramsPM.xlsx
+++ b/aqpolypy/salt/paramsPM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trvsst\Research\aqpolypy\aqpolypy\salt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFFC7F0-E012-401A-AD14-2CCD20D8DE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFEEB7A-26E0-43DD-B180-54C7BFCC2366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>HCl</t>
   </si>
@@ -297,15 +297,6 @@
     <t>LipTolueneS</t>
   </si>
   <si>
-    <t>NapToluene</t>
-  </si>
-  <si>
-    <t>KpToluene</t>
-  </si>
-  <si>
-    <t>2,5Me2BenzeneS</t>
-  </si>
-  <si>
     <t>Li2,5Me2BenzeneS</t>
   </si>
   <si>
@@ -400,6 +391,18 @@
   </si>
   <si>
     <t>Pr4NF</t>
+  </si>
+  <si>
+    <t>pTolueneSA</t>
+  </si>
+  <si>
+    <t>NapTolueneS</t>
+  </si>
+  <si>
+    <t>KpTolueneS</t>
+  </si>
+  <si>
+    <t>2,5Me2BenzeneSA</t>
   </si>
 </sst>
 </file>
@@ -717,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -730,31 +733,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>111</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>114</v>
-      </c>
-      <c r="G1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1339,7 +1342,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B22">
         <v>-5.33E-2</v>
@@ -1513,7 +1516,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B28">
         <v>7.46E-2</v>
@@ -1774,7 +1777,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B37">
         <v>2.69E-2</v>
@@ -2499,7 +2502,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B62">
         <v>0.44629999999999997</v>
@@ -2879,7 +2882,7 @@
         <v>69</v>
       </c>
       <c r="B75">
-        <v>0.78700000000000003</v>
+        <v>7.8700000000000006E-2</v>
       </c>
       <c r="C75">
         <v>0.27400000000000002</v>
@@ -3198,7 +3201,7 @@
         <v>80</v>
       </c>
       <c r="B86">
-        <v>0.1792</v>
+        <v>0.17960000000000001</v>
       </c>
       <c r="C86">
         <v>8.3000000000000004E-2</v>
@@ -3262,7 +3265,7 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="D88">
-        <v>3.5999999999999999E-3</v>
+        <v>-3.7400000000000003E-2</v>
       </c>
       <c r="E88">
         <v>4</v>
@@ -3369,19 +3372,19 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="B92">
-        <v>1.89E-2</v>
+        <v>-3.6600000000000001E-2</v>
       </c>
       <c r="C92">
-        <v>0.39900000000000002</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="D92">
-        <v>4.5999999999999999E-3</v>
+        <v>1.37E-2</v>
       </c>
       <c r="E92">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -3398,19 +3401,19 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B93">
-        <v>-3.44E-2</v>
+        <v>1.89E-2</v>
       </c>
       <c r="C93">
-        <v>0.39600000000000002</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="D93">
-        <v>4.3E-3</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="E93">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -3427,19 +3430,19 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="B94">
-        <v>-9.8500000000000004E-2</v>
+        <v>-3.44E-2</v>
       </c>
       <c r="C94">
-        <v>0.45300000000000001</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="D94">
-        <v>1.2200000000000001E-2</v>
+        <v>4.3E-3</v>
       </c>
       <c r="E94">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -3456,19 +3459,19 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="B95">
-        <v>-9.6500000000000002E-2</v>
+        <v>-9.8500000000000004E-2</v>
       </c>
       <c r="C95">
-        <v>0.14099999999999999</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="D95">
-        <v>2.1000000000000001E-2</v>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="E95">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -3485,19 +3488,19 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="B96">
-        <v>-9.7999999999999997E-3</v>
+        <v>-9.6500000000000002E-2</v>
       </c>
       <c r="C96">
-        <v>0.36099999999999999</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D96">
-        <v>3.8999999999999998E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="E96">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -3514,19 +3517,19 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B97">
-        <v>-0.1736</v>
+        <v>-9.7999999999999997E-3</v>
       </c>
       <c r="C97">
-        <v>0.435</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="D97">
-        <v>3.8300000000000001E-2</v>
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="E97">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -3543,19 +3546,19 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B98">
-        <v>-0.14380000000000001</v>
+        <v>-0.1736</v>
       </c>
       <c r="C98">
-        <v>0.80400000000000005</v>
+        <v>0.435</v>
       </c>
       <c r="D98">
-        <v>3.1699999999999999E-2</v>
+        <v>3.8300000000000001E-2</v>
       </c>
       <c r="E98">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -3572,19 +3575,19 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B99">
-        <v>-0.224</v>
+        <v>-0.14380000000000001</v>
       </c>
       <c r="C99">
-        <v>0.89500000000000002</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="D99">
-        <v>3.5499999999999997E-2</v>
+        <v>3.1699999999999999E-2</v>
       </c>
       <c r="E99">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -3601,19 +3604,19 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B100">
-        <v>-0.22090000000000001</v>
+        <v>-0.224</v>
       </c>
       <c r="C100">
-        <v>0.248</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="D100">
-        <v>4.3200000000000002E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="E100">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -3630,16 +3633,16 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B101">
-        <v>-0.1198</v>
+        <v>-0.22090000000000001</v>
       </c>
       <c r="C101">
-        <v>0.871</v>
+        <v>0.248</v>
       </c>
       <c r="D101">
-        <v>4.5620000000000001E-2</v>
+        <v>4.3200000000000002E-2</v>
       </c>
       <c r="E101">
         <v>2</v>
@@ -3659,19 +3662,19 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B102">
-        <v>4.5699999999999998E-2</v>
+        <v>-0.1198</v>
       </c>
       <c r="C102">
-        <v>-0.19600000000000001</v>
+        <v>0.871</v>
       </c>
       <c r="D102">
-        <v>8.0000000000000004E-4</v>
+        <v>4.5620000000000001E-2</v>
       </c>
       <c r="E102">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -3688,16 +3691,16 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B103">
-        <v>-6.6E-3</v>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="C103">
-        <v>-0.22700000000000001</v>
+        <v>-0.19600000000000001</v>
       </c>
       <c r="D103">
-        <v>3.5999999999999999E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E103">
         <v>6</v>
@@ -3717,19 +3720,19 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B104">
-        <v>-8.2100000000000006E-2</v>
+        <v>-6.6E-3</v>
       </c>
       <c r="C104">
-        <v>-0.17799999999999999</v>
+        <v>-0.22700000000000001</v>
       </c>
       <c r="D104">
-        <v>1.6199999999999999E-2</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E104">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3746,19 +3749,19 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B105">
-        <v>-0.1517</v>
+        <v>-8.2100000000000006E-2</v>
       </c>
       <c r="C105">
-        <v>-0.54500000000000004</v>
+        <v>-0.17799999999999999</v>
       </c>
       <c r="D105">
-        <v>1.8700000000000001E-2</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="E105">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3775,19 +3778,19 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B106">
-        <v>-8.7900000000000006E-2</v>
+        <v>-0.1517</v>
       </c>
       <c r="C106">
-        <v>-0.34300000000000003</v>
+        <v>-0.54500000000000004</v>
       </c>
       <c r="D106">
-        <v>1.34E-2</v>
+        <v>1.8700000000000001E-2</v>
       </c>
       <c r="E106">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3804,19 +3807,19 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B107">
-        <v>-0.15179999999999999</v>
+        <v>-8.7900000000000006E-2</v>
       </c>
       <c r="C107">
-        <v>-0.77800000000000002</v>
+        <v>-0.34300000000000003</v>
       </c>
       <c r="D107">
-        <v>1.77E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="E107">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -3833,19 +3836,19 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B108">
-        <v>9.3799999999999994E-2</v>
+        <v>-0.15179999999999999</v>
       </c>
       <c r="C108">
-        <v>0.128</v>
+        <v>-0.77800000000000002</v>
       </c>
       <c r="D108">
-        <v>-3.0000000000000001E-3</v>
+        <v>1.77E-2</v>
       </c>
       <c r="E108">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -3862,19 +3865,19 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B109">
-        <v>-4.7399999999999998E-2</v>
+        <v>9.3799999999999994E-2</v>
       </c>
       <c r="C109">
-        <v>-0.25900000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="D109">
-        <v>1.06E-2</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="E109">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -3891,19 +3894,19 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B110">
-        <v>3.1399999999999997E-2</v>
+        <v>-4.7399999999999998E-2</v>
       </c>
       <c r="C110">
-        <v>-0.184</v>
+        <v>-0.25900000000000001</v>
       </c>
       <c r="D110">
-        <v>2.3E-3</v>
+        <v>1.06E-2</v>
       </c>
       <c r="E110">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -3920,16 +3923,16 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B111">
-        <v>-2.2800000000000001E-2</v>
+        <v>3.1399999999999997E-2</v>
       </c>
       <c r="C111">
-        <v>-0.245</v>
+        <v>-0.184</v>
       </c>
       <c r="D111">
-        <v>4.4000000000000003E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="E111">
         <v>6</v>
@@ -3949,19 +3952,19 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B112">
-        <v>-0.60099999999999998</v>
+        <v>-2.2800000000000001E-2</v>
       </c>
       <c r="C112">
-        <v>-0.60399999999999998</v>
+        <v>-0.245</v>
       </c>
       <c r="D112">
-        <v>6.0000000000000001E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="E112">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -3978,19 +3981,19 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B113">
-        <v>7.2599999999999998E-2</v>
+        <v>-6.0100000000000001E-2</v>
       </c>
       <c r="C113">
-        <v>-0.245</v>
+        <v>-0.60399999999999998</v>
       </c>
       <c r="D113">
-        <v>-9.9000000000000008E-3</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="E113">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -4007,16 +4010,16 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B114">
-        <v>-8.0299999999999996E-2</v>
+        <v>7.2599999999999998E-2</v>
       </c>
       <c r="C114">
-        <v>-0.61599999999999999</v>
+        <v>-0.245</v>
       </c>
       <c r="D114">
-        <v>5.3E-3</v>
+        <v>-9.9000000000000008E-3</v>
       </c>
       <c r="E114">
         <v>6</v>
@@ -4031,6 +4034,35 @@
         <v>1</v>
       </c>
       <c r="I114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>105</v>
+      </c>
+      <c r="B115">
+        <v>-8.0299999999999996E-2</v>
+      </c>
+      <c r="C115">
+        <v>-0.61599999999999999</v>
+      </c>
+      <c r="D115">
+        <v>5.3E-3</v>
+      </c>
+      <c r="E115">
+        <v>6</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="G115">
+        <v>-1</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
         <v>1</v>
       </c>
     </row>

</xml_diff>